<commit_message>
Deploying to gh-pages from @ Healthedata1/R5ElementExtensionTest@ccecc9c1bcbd8e3897c57e11237e24b03def5e78 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-medicationstatement.xlsx
+++ b/StructureDefinition-us-core-medicationstatement.xlsx
@@ -27,7 +27,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://www.fhir.org/guides/uscdi4-sandbox/StructureDefinition/us-core-medicationstatement</t>
+    <t>http://www.fhir.org/guides/testing-sandbox/StructureDefinition/us-core-medicationstatement</t>
   </si>
   <si>
     <t>Version</t>
@@ -468,7 +468,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>http://www.fhir.org/guides/uscdi4-sandbox/ValueSet/uscore-medicationstatement-status</t>
+    <t>http://www.fhir.org/guides/testing-sandbox/ValueSet/uscore-medicationstatement-status</t>
   </si>
   <si>
     <t>Event.status</t>
@@ -1572,7 +1572,7 @@
     <col min="23" max="23" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="10.53125" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="198.02734375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="82.328125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="82.71875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="10.26171875" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>

</xml_diff>